<commit_message>
major milestone 3 docs
</commit_message>
<xml_diff>
--- a/Milestone 3 Documentation/Milestone 3 Master-Rubric-Review.xlsx
+++ b/Milestone 3 Documentation/Milestone 3 Master-Rubric-Review.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24617"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/victoriakokurin/GitHub/A-Slight-Sep-Up/Milestone 3 Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E57DDCD8-80F9-2A4F-BCC6-169A9CBC2249}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="40" documentId="13_ncr:1_{E57DDCD8-80F9-2A4F-BCC6-169A9CBC2249}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B31BBF1A-27A2-4147-8DC3-BBF086979729}"/>
   <bookViews>
     <workbookView xWindow="-36920" yWindow="3180" windowWidth="33820" windowHeight="16960" xr2:uid="{439F960B-B781-BC40-B75C-C9C74F21A181}"/>
   </bookViews>
@@ -78,46 +78,76 @@
     <t>1. All features that have been promised through sprint planning of sprints 1 and 2 have been implemented and validated.</t>
   </si>
   <si>
+    <t xml:space="preserve">Clean up Jira &amp; Validate the sprint in the sprint retro(what has been/hasn’t been done) - Kyrice </t>
+  </si>
+  <si>
     <t>1. Sessions have been managed through JWT.</t>
   </si>
   <si>
+    <t xml:space="preserve">2. All weekly meetings attended, with all members regularly present, evidence of more than 2 weekly standups per week, evidence of regular communications (at least every second day) between team members, meeting minutes, including action items. </t>
+  </si>
+  <si>
+    <t>Meeting minutes for 9 meetings + Screenshots of regular communication - Nandini</t>
+  </si>
+  <si>
+    <t>2. All sprint activities have been done and documented with no error.</t>
+  </si>
+  <si>
+    <t>Sprint retro x2 (sprint 2 &amp; 3) , sprint planning x1 (sprint 3) (could do hypotherical spring 4 document) - Noel</t>
+  </si>
+  <si>
+    <t>3. Professional use of branching in Git-based on each task, proper organisation of Jira board following one of the proposed templates, evidence of proper Sprint planning, frequent commits and Trello task status updates, consistent appropriate commit messages.</t>
+  </si>
+  <si>
+    <t>Trello (vica) and Jira (Kyrice) evidence of backlog grooming (document)</t>
+  </si>
+  <si>
+    <t>3. CircleCI for CI/CD. Ci yml has no error and the dockerised application has been built with no error on CI machine.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vica - more screenshots </t>
+  </si>
+  <si>
+    <t>3. Evidence of backlog grooming after each sprint</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kyrice - Jira </t>
+  </si>
+  <si>
+    <t>3. Evidence of iterative and incremental implementation ( not scrumfall). The velocity of the teamwork is not negative</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kyriece - Burndown chart </t>
+  </si>
+  <si>
+    <t>4. Flawless code styling/organisation and comments, following the code structure and architecture</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Create a new comment branch and everyone picks an area to cover - Noel (loginmicroservices), Kyriece (Books + bookmicroservices), Vica (information + requestsmicroservices, user management, docker files and circleci), Nandini - frontend design </t>
+  </si>
+  <si>
+    <t xml:space="preserve">4. the appropriate number of User Stories per feature, No Epic. </t>
+  </si>
+  <si>
+    <t>4. User Stories are properly structured and complete and comprehensive</t>
+  </si>
+  <si>
+    <t>4. No linting issue code, docker file or yml file.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vica </t>
+  </si>
+  <si>
+    <t>5. Comprehensive Unit and Acceptance Tests (for all features), tests demonstrating both positive, negative and boundary testing,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Noel + screenshot of tests passing </t>
+  </si>
+  <si>
+    <t>5.  Acceptance tests appropriately constructed from User Stories, evidence of testing properly documented</t>
+  </si>
+  <si>
     <t>tim</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2. All weekly meetings attended, with all members regularly present, evidence of more than 2 weekly standups per week, evidence of regular communications (at least every second day) between team members, meeting minutes, including action items. </t>
-  </si>
-  <si>
-    <t>2. All sprint activities have been done and documented with no error.</t>
-  </si>
-  <si>
-    <t>3. Professional use of branching in Git-based on each task, proper organisation of Jira board following one of the proposed templates, evidence of proper Sprint planning, frequent commits and Trello task status updates, consistent appropriate commit messages.</t>
-  </si>
-  <si>
-    <t>3. CircleCI for CI/CD. Ci yml has no error and the dockerised application has been built with no error on CI machine.</t>
-  </si>
-  <si>
-    <t>3. Evidence of backlog grooming after each sprint</t>
-  </si>
-  <si>
-    <t>3. Evidence of iterative and incremental implementation ( not scrumfall). The velocity of the teamwork is not negative</t>
-  </si>
-  <si>
-    <t>4. Flawless code styling/organisation and comments, following the code structure and architecture</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4. the appropriate number of User Stories per feature, No Epic. </t>
-  </si>
-  <si>
-    <t>4. User Stories are properly structured and complete and comprehensive</t>
-  </si>
-  <si>
-    <t>4. No linting issue code, docker file or yml file.</t>
-  </si>
-  <si>
-    <t>5. Comprehensive Unit and Acceptance Tests (for all features), tests demonstrating both positive, negative and boundary testing,</t>
-  </si>
-  <si>
-    <t>5.  Acceptance tests appropriately constructed from User Stories, evidence of testing properly documented</t>
   </si>
   <si>
     <t>other admin tasks</t>
@@ -135,42 +165,12 @@
 a diagram of your Deployment pipeline setup: i.e,. CI/CD, steps in the pipeline, automation tools in the pipeline
 documentation of acceptance test cases and evidence of test execution (when they were run; pass/fail status of each run)</t>
   </si>
-  <si>
-    <t xml:space="preserve">Clean up Jira &amp; Validate the sprint in the sprint retro(what has been/hasn’t been done) - Kyrice </t>
-  </si>
-  <si>
-    <t>Meeting minutes for 9 meetings + Screenshots of regular communication - Nandini</t>
-  </si>
-  <si>
-    <t>Sprint retro x2 (sprint 2 &amp; 3) , sprint planning x1 (sprint 3) (could do hypotherical spring 4 document) - Noel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vica - more screenshots </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kyrice - Jira </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kyriece - Burndown chart </t>
-  </si>
-  <si>
-    <t>Trello (vica) and Jira (Kyrice) evidence of backlog grooming (document)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Create a new comment branch and everyone picks an area to cover - Noel (loginmicroservices), Kyriece (Books + bookmicroservices), Vica (information + requestsmicroservices, user management, docker files and circleci), Nandini - frontend design </t>
-  </si>
-  <si>
-    <t xml:space="preserve">vica </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Noel + screenshot of tests passing </t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -236,7 +236,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -257,6 +257,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -575,33 +578,33 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C87E0E4-888A-E84E-AE5C-42B7977AFF61}">
   <dimension ref="A1:C27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.95"/>
   <cols>
-    <col min="1" max="1" width="57.33203125" style="1" customWidth="1"/>
-    <col min="2" max="3" width="43.33203125" style="1" customWidth="1"/>
-    <col min="4" max="16384" width="10.83203125" style="1"/>
+    <col min="1" max="1" width="57.375" style="1" customWidth="1"/>
+    <col min="2" max="3" width="43.375" style="1" customWidth="1"/>
+    <col min="4" max="16384" width="10.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" ht="17.100000000000001">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="170" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" ht="170.1">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="187" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" ht="186.95">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:3" s="3" customFormat="1" ht="221" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" s="3" customFormat="1" ht="221.1">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
@@ -612,17 +615,17 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:3" s="3" customFormat="1" ht="153" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" s="3" customFormat="1" ht="153">
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:3" s="3" customFormat="1" ht="102" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" s="3" customFormat="1" ht="60">
       <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:3" s="4" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" s="4" customFormat="1" ht="17.100000000000001">
       <c r="A7" s="4" t="s">
         <v>8</v>
       </c>
@@ -633,153 +636,153 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="85" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" ht="84.95">
       <c r="A8" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B8" s="7"/>
     </row>
-    <row r="9" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" ht="33.950000000000003">
       <c r="A9" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B9" s="7"/>
     </row>
-    <row r="10" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" ht="33.950000000000003">
       <c r="A10" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B10" s="6"/>
       <c r="C10" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="17.100000000000001">
       <c r="A11" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B11" s="7"/>
     </row>
-    <row r="12" spans="1:3" ht="68" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" ht="68.099999999999994">
       <c r="A12" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="6"/>
+      <c r="B12" s="4"/>
       <c r="C12" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="51" x14ac:dyDescent="0.2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="47.25">
       <c r="A13" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B13" s="5"/>
+        <v>18</v>
+      </c>
+      <c r="B13" s="8"/>
       <c r="C13" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="85" x14ac:dyDescent="0.2">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="63">
       <c r="A14" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B14" s="5"/>
       <c r="C14" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="33.950000000000003">
       <c r="A15" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B15" s="5"/>
+        <v>22</v>
+      </c>
+      <c r="B15" s="8"/>
       <c r="C15" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="17.100000000000001">
       <c r="A16" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B16" s="6"/>
+        <v>24</v>
+      </c>
+      <c r="B16" s="4"/>
       <c r="C16" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="31.5">
       <c r="A17" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B17" s="5"/>
+        <v>26</v>
+      </c>
+      <c r="B17" s="8"/>
       <c r="C17" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="102" x14ac:dyDescent="0.2">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="78.75">
       <c r="A18" s="1" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="B18" s="5"/>
       <c r="C18" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="17.100000000000001">
+      <c r="A19" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B19" s="7"/>
+    </row>
+    <row r="20" spans="1:3" ht="33.950000000000003">
+      <c r="A20" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B20" s="7"/>
+    </row>
+    <row r="21" spans="1:3" ht="15.75">
+      <c r="A21" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B21" s="4"/>
+      <c r="C21" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="31.5">
+      <c r="A22" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B22" s="8"/>
+      <c r="C22" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="51">
+      <c r="A23" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B23" s="8"/>
+      <c r="C23" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="17.100000000000001">
+      <c r="A24" s="1" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A19" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B19" s="7"/>
-    </row>
-    <row r="20" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A20" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B20" s="7"/>
-    </row>
-    <row r="21" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A21" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B21" s="6"/>
-      <c r="C21" s="1" t="s">
+      <c r="B24" s="5"/>
+    </row>
+    <row r="25" spans="1:3" ht="17.100000000000001">
+      <c r="A25" s="1" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A22" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B22" s="5"/>
-      <c r="C22" s="1" t="s">
+      <c r="B25" s="8"/>
+      <c r="C25" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="306">
+      <c r="A27" s="1" t="s">
         <v>40</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" ht="51" x14ac:dyDescent="0.2">
-      <c r="A23" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B23" s="5"/>
-      <c r="C23" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A24" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B24" s="5"/>
-    </row>
-    <row r="25" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A25" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B25" s="5"/>
-      <c r="C25" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" ht="306" x14ac:dyDescent="0.2">
-      <c r="A27" s="1" t="s">
-        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -788,18 +791,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -975,36 +978,13 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DD8438FB-FF8B-46AB-BE4F-1226DF4BE235}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7F43504D-8E16-4841-BD6C-9CC71557A02A}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7F43504D-8E16-4841-BD6C-9CC71557A02A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DD8438FB-FF8B-46AB-BE4F-1226DF4BE235}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9F29E129-0A28-4715-8753-F53F5A82E660}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="1977bc59-59cf-46de-bb10-abef6dc3255c"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9F29E129-0A28-4715-8753-F53F5A82E660}"/>
 </file>
</xml_diff>